<commit_message>
1) add new API 1.31.3.26-2 for Reader 2) change to one simple plan for Reader and switch the twp plans 3) read tag Timer change to 2s
</commit_message>
<xml_diff>
--- a/doc/PTMS_RDM_Modbus_V1.0.1.xlsx
+++ b/doc/PTMS_RDM_Modbus_V1.0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="协议说明" sheetId="7" r:id="rId1"/>
@@ -1167,47 +1167,53 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1216,12 +1222,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1766,16 +1766,16 @@
       </c>
     </row>
     <row r="7" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="E7" s="46">
+      <c r="E7" s="48">
         <v>1</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="46" t="s">
         <v>120</v>
       </c>
       <c r="G7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="46" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="8" t="s">
@@ -1786,10 +1786,10 @@
       </c>
     </row>
     <row r="8" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="E8" s="47"/>
-      <c r="F8" s="53"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="47"/>
       <c r="G8" s="51"/>
-      <c r="H8" s="53"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1985,16 +1985,16 @@
       <c r="J18" s="12"/>
     </row>
     <row r="19" spans="5:10" ht="17.25" customHeight="1">
-      <c r="E19" s="46">
+      <c r="E19" s="48">
         <v>12</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F19" s="52" t="s">
         <v>134</v>
       </c>
       <c r="G19" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="46" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="8" t="s">
@@ -2005,10 +2005,10 @@
       </c>
     </row>
     <row r="20" spans="5:10" ht="19.5" customHeight="1">
-      <c r="E20" s="47"/>
-      <c r="F20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="53"/>
       <c r="G20" s="51"/>
-      <c r="H20" s="53"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="6" t="s">
         <v>161</v>
       </c>
@@ -2017,16 +2017,16 @@
       </c>
     </row>
     <row r="21" spans="5:10" ht="13.5" customHeight="1">
-      <c r="E21" s="46">
+      <c r="E21" s="48">
         <v>13</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="52" t="s">
         <v>177</v>
       </c>
       <c r="G21" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="H21" s="52" t="s">
+      <c r="H21" s="46" t="s">
         <v>3</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -2037,10 +2037,10 @@
       </c>
     </row>
     <row r="22" spans="5:10" ht="17.25" customHeight="1">
-      <c r="E22" s="47"/>
-      <c r="F22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="53"/>
       <c r="G22" s="51"/>
-      <c r="H22" s="53"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="6" t="s">
         <v>169</v>
       </c>
@@ -2049,16 +2049,16 @@
       </c>
     </row>
     <row r="23" spans="5:10" ht="20.100000000000001" customHeight="1">
-      <c r="E23" s="46">
+      <c r="E23" s="48">
         <v>14</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="52" t="s">
         <v>178</v>
       </c>
       <c r="G23" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="46" t="s">
         <v>3</v>
       </c>
       <c r="I23" s="8" t="s">
@@ -2069,10 +2069,10 @@
       </c>
     </row>
     <row r="24" spans="5:10" ht="15.75" customHeight="1">
-      <c r="E24" s="47"/>
-      <c r="F24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="53"/>
       <c r="G24" s="51"/>
-      <c r="H24" s="53"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="6" t="s">
         <v>164</v>
       </c>
@@ -2082,6 +2082,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
@@ -2090,14 +2098,6 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="H19:H20"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2108,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2145,16 +2145,16 @@
       </c>
     </row>
     <row r="7" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="C7" s="63">
+      <c r="C7" s="54">
         <v>1</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="56" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="23" t="s">
@@ -2163,26 +2163,26 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="C8" s="64"/>
-      <c r="D8" s="56"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="59"/>
-      <c r="F8" s="56"/>
+      <c r="F8" s="57"/>
       <c r="G8" s="24" t="s">
         <v>165</v>
       </c>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="C9" s="63">
+      <c r="C9" s="54">
         <v>2</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="56" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="23" t="s">
@@ -2191,26 +2191,26 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="C10" s="64"/>
-      <c r="D10" s="56"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="57"/>
       <c r="E10" s="59"/>
-      <c r="F10" s="56"/>
+      <c r="F10" s="57"/>
       <c r="G10" s="24" t="s">
         <v>157</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="C11" s="63">
+      <c r="C11" s="54">
         <v>3</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="F11" s="54" t="s">
+      <c r="F11" s="56" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="23" t="s">
@@ -2219,10 +2219,10 @@
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="3:10" ht="20.100000000000001" customHeight="1">
-      <c r="C12" s="64"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="59"/>
-      <c r="F12" s="56"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="24" t="s">
         <v>159</v>
       </c>
@@ -2705,292 +2705,292 @@
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="3:8">
-      <c r="C39" s="54">
+      <c r="C39" s="56">
         <v>30</v>
       </c>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="57" t="s">
+      <c r="E39" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="54" t="s">
+      <c r="F39" s="56" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="60"/>
+      <c r="H39" s="62"/>
     </row>
     <row r="40" spans="3:8">
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="55"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="60"/>
       <c r="G40" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H40" s="61"/>
+      <c r="H40" s="63"/>
     </row>
     <row r="41" spans="3:8">
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="55"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="60"/>
       <c r="G41" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="61"/>
+      <c r="H41" s="63"/>
     </row>
     <row r="42" spans="3:8">
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
       <c r="E42" s="59"/>
-      <c r="F42" s="56"/>
+      <c r="F42" s="57"/>
       <c r="G42" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="62"/>
+      <c r="H42" s="64"/>
     </row>
     <row r="43" spans="3:8">
-      <c r="C43" s="54">
+      <c r="C43" s="56">
         <v>31</v>
       </c>
-      <c r="D43" s="54" t="s">
+      <c r="D43" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="E43" s="57" t="s">
+      <c r="E43" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="F43" s="54" t="s">
+      <c r="F43" s="56" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H43" s="60"/>
+      <c r="H43" s="62"/>
     </row>
     <row r="44" spans="3:8">
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="55"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="60"/>
       <c r="G44" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H44" s="61"/>
+      <c r="H44" s="63"/>
     </row>
     <row r="45" spans="3:8">
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="55"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="60"/>
       <c r="G45" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H45" s="61"/>
+      <c r="H45" s="63"/>
     </row>
     <row r="46" spans="3:8">
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
       <c r="E46" s="59"/>
-      <c r="F46" s="56"/>
+      <c r="F46" s="57"/>
       <c r="G46" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="62"/>
+      <c r="H46" s="64"/>
     </row>
     <row r="47" spans="3:8">
-      <c r="C47" s="54">
+      <c r="C47" s="56">
         <v>32</v>
       </c>
-      <c r="D47" s="54" t="s">
+      <c r="D47" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="F47" s="54" t="s">
+      <c r="F47" s="56" t="s">
         <v>9</v>
       </c>
       <c r="G47" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="60"/>
+      <c r="H47" s="62"/>
     </row>
     <row r="48" spans="3:8">
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="55"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="60"/>
       <c r="G48" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="61"/>
+      <c r="H48" s="63"/>
     </row>
     <row r="49" spans="3:8">
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="55"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="60"/>
       <c r="G49" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="61"/>
+      <c r="H49" s="63"/>
     </row>
     <row r="50" spans="3:8">
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
       <c r="E50" s="59"/>
-      <c r="F50" s="56"/>
+      <c r="F50" s="57"/>
       <c r="G50" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="62"/>
+      <c r="H50" s="64"/>
     </row>
     <row r="51" spans="3:8">
-      <c r="C51" s="54">
+      <c r="C51" s="56">
         <v>33</v>
       </c>
-      <c r="D51" s="54" t="s">
+      <c r="D51" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="E51" s="57" t="s">
+      <c r="E51" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="F51" s="54" t="s">
+      <c r="F51" s="56" t="s">
         <v>9</v>
       </c>
       <c r="G51" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H51" s="60"/>
+      <c r="H51" s="62"/>
     </row>
     <row r="52" spans="3:8">
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="55"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="60"/>
       <c r="G52" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H52" s="61"/>
+      <c r="H52" s="63"/>
     </row>
     <row r="53" spans="3:8">
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="55"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="60"/>
       <c r="G53" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H53" s="61"/>
+      <c r="H53" s="63"/>
     </row>
     <row r="54" spans="3:8">
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
       <c r="E54" s="59"/>
-      <c r="F54" s="56"/>
+      <c r="F54" s="57"/>
       <c r="G54" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H54" s="62"/>
+      <c r="H54" s="64"/>
     </row>
     <row r="55" spans="3:8">
-      <c r="C55" s="54">
+      <c r="C55" s="56">
         <v>34</v>
       </c>
-      <c r="D55" s="54" t="s">
+      <c r="D55" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="E55" s="57" t="s">
+      <c r="E55" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="F55" s="54" t="s">
+      <c r="F55" s="56" t="s">
         <v>9</v>
       </c>
       <c r="G55" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H55" s="60"/>
+      <c r="H55" s="62"/>
     </row>
     <row r="56" spans="3:8">
-      <c r="C56" s="55"/>
-      <c r="D56" s="55"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="55"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="61"/>
+      <c r="F56" s="60"/>
       <c r="G56" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H56" s="61"/>
+      <c r="H56" s="63"/>
     </row>
     <row r="57" spans="3:8">
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="55"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="60"/>
       <c r="G57" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H57" s="61"/>
+      <c r="H57" s="63"/>
     </row>
     <row r="58" spans="3:8">
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
       <c r="E58" s="59"/>
-      <c r="F58" s="56"/>
+      <c r="F58" s="57"/>
       <c r="G58" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H58" s="62"/>
+      <c r="H58" s="64"/>
     </row>
     <row r="59" spans="3:8">
-      <c r="C59" s="54">
+      <c r="C59" s="56">
         <v>35</v>
       </c>
-      <c r="D59" s="54" t="s">
+      <c r="D59" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="E59" s="57" t="s">
+      <c r="E59" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="F59" s="54" t="s">
+      <c r="F59" s="56" t="s">
         <v>9</v>
       </c>
       <c r="G59" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H59" s="60"/>
+      <c r="H59" s="62"/>
     </row>
     <row r="60" spans="3:8">
-      <c r="C60" s="55"/>
-      <c r="D60" s="55"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="55"/>
+      <c r="C60" s="60"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="60"/>
       <c r="G60" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H60" s="61"/>
+      <c r="H60" s="63"/>
     </row>
     <row r="61" spans="3:8">
-      <c r="C61" s="55"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="55"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="61"/>
+      <c r="F61" s="60"/>
       <c r="G61" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H61" s="61"/>
+      <c r="H61" s="63"/>
     </row>
     <row r="62" spans="3:8">
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
       <c r="E62" s="59"/>
-      <c r="F62" s="56"/>
+      <c r="F62" s="57"/>
       <c r="G62" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H62" s="62"/>
+      <c r="H62" s="64"/>
     </row>
     <row r="63" spans="3:8" ht="54.75" customHeight="1">
       <c r="C63" s="30">
@@ -3003,58 +3003,58 @@
         <v>222</v>
       </c>
       <c r="F63" s="28" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G63" s="24"/>
       <c r="H63" s="22"/>
     </row>
     <row r="64" spans="3:8">
-      <c r="C64" s="54">
+      <c r="C64" s="56">
         <v>37</v>
       </c>
-      <c r="D64" s="54" t="s">
+      <c r="D64" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="E64" s="57" t="s">
+      <c r="E64" s="58" t="s">
         <v>217</v>
       </c>
-      <c r="F64" s="54" t="s">
+      <c r="F64" s="56" t="s">
         <v>9</v>
       </c>
       <c r="G64" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H64" s="60"/>
+      <c r="H64" s="62"/>
     </row>
     <row r="65" spans="3:8">
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="55"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="61"/>
+      <c r="F65" s="60"/>
       <c r="G65" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H65" s="61"/>
+      <c r="H65" s="63"/>
     </row>
     <row r="66" spans="3:8">
-      <c r="C66" s="55"/>
-      <c r="D66" s="55"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="55"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="60"/>
       <c r="G66" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H66" s="61"/>
+      <c r="H66" s="63"/>
     </row>
     <row r="67" spans="3:8">
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
       <c r="E67" s="59"/>
-      <c r="F67" s="56"/>
+      <c r="F67" s="57"/>
       <c r="G67" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="62"/>
+      <c r="H67" s="64"/>
     </row>
     <row r="68" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C68" s="5">
@@ -3205,6 +3205,41 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="F47:F50"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="F59:F62"/>
+    <mergeCell ref="H59:H62"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="F55:F58"/>
+    <mergeCell ref="H55:H58"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="H64:H67"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
@@ -3217,41 +3252,6 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="H64:H67"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="F55:F58"/>
-    <mergeCell ref="H55:H58"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="F59:F62"/>
-    <mergeCell ref="H59:H62"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="F47:F50"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="H51:H54"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="H43:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3453,7 +3453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>